<commit_message>
Fiddle with univariate model summary spreadsheet:
</commit_message>
<xml_diff>
--- a/model-summary-for-Tony.xlsx
+++ b/model-summary-for-Tony.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6A20217E-5B09-584B-AB9D-B8531D06E2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FA508-B2D3-454F-8D07-180AD22712F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="960" windowWidth="27700" windowHeight="16040"/>
+    <workbookView xWindow="740" yWindow="960" windowWidth="14620" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model-summary-for-Tony" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -131,13 +131,25 @@
   </si>
   <si>
     <t>Model response</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,6 +271,12 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
@@ -604,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -613,6 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -967,11 +986,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -985,7 +1004,7 @@
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1007,7 +1026,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="D2" t="s">
         <v>31</v>
       </c>
@@ -1021,7 +1040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1046,8 +1065,11 @@
       <c r="H4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -1069,8 +1091,11 @@
       <c r="H5" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1092,8 +1117,11 @@
       <c r="H6" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -1115,8 +1143,11 @@
       <c r="H7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -1138,8 +1169,11 @@
       <c r="H8" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1196,7 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1184,8 +1218,11 @@
       <c r="H10" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1207,8 +1244,11 @@
       <c r="H11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1271,7 @@
         <v>0.40799999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1254,7 +1294,7 @@
         <v>0.11799999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1277,7 +1317,7 @@
         <v>0.48799999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1299,8 +1339,11 @@
       <c r="H15" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1323,10 +1366,10 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1351,8 +1394,11 @@
       <c r="H18" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -1374,8 +1420,11 @@
       <c r="H19" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1397,8 +1446,11 @@
       <c r="H20" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1421,7 +1473,7 @@
         <v>0.57699999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:9">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -1444,7 +1496,7 @@
         <v>0.34899999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -1466,8 +1518,11 @@
       <c r="H23" s="1">
         <v>0.10299999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="B24" t="s">
         <v>4</v>
       </c>
@@ -1489,8 +1544,11 @@
       <c r="H24" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="B25" t="s">
         <v>5</v>
       </c>
@@ -1512,8 +1570,11 @@
       <c r="H25" s="1">
         <v>7.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="B26" t="s">
         <v>6</v>
       </c>
@@ -1536,7 +1597,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:9">
       <c r="B27" t="s">
         <v>7</v>
       </c>
@@ -1558,8 +1619,11 @@
       <c r="H27" s="1">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -1582,7 +1646,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="B29" t="s">
         <v>11</v>
       </c>
@@ -1605,7 +1669,7 @@
         <v>0.28699999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="B30" t="s">
         <v>18</v>
       </c>
@@ -1628,7 +1692,7 @@
         <v>0.27800000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="B31" t="s">
         <v>19</v>
       </c>
@@ -1651,7 +1715,7 @@
         <v>0.249</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>12</v>
       </c>
@@ -1673,8 +1737,11 @@
       <c r="H32" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="B33" t="s">
         <v>13</v>
       </c>
@@ -1697,10 +1764,10 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:9">
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1725,8 +1792,11 @@
       <c r="H35" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -1748,8 +1818,11 @@
       <c r="H36" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="B37" t="s">
         <v>21</v>
       </c>
@@ -1771,8 +1844,11 @@
       <c r="H37" s="1">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -1794,8 +1870,11 @@
       <c r="H38" s="1">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="B39" t="s">
         <v>16</v>
       </c>
@@ -1817,8 +1896,11 @@
       <c r="H39" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>17</v>
       </c>
@@ -1841,7 +1923,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
         <v>6</v>
       </c>
@@ -1863,8 +1945,11 @@
       <c r="H41" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="B42" t="s">
         <v>7</v>
       </c>
@@ -1887,7 +1972,7 @@
         <v>0.191</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:9">
       <c r="B43" t="s">
         <v>22</v>
       </c>
@@ -1909,8 +1994,11 @@
       <c r="H43" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="B44" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +2021,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:9">
       <c r="B45" t="s">
         <v>24</v>
       </c>
@@ -1955,8 +2043,11 @@
       <c r="H45" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="B46" t="s">
         <v>25</v>
       </c>
@@ -1978,8 +2069,11 @@
       <c r="H46" s="1">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="B47" t="s">
         <v>12</v>
       </c>
@@ -2001,8 +2095,11 @@
       <c r="H47" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="B48" t="s">
         <v>13</v>
       </c>
@@ -2030,6 +2127,42 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:C33">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:C48">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>